<commit_message>
feat: import excel student
</commit_message>
<xml_diff>
--- a/public/assets/files/templates/teacher.xlsx
+++ b/public/assets/files/templates/teacher.xlsx
@@ -37,34 +37,34 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">wildan</t>
+    <t xml:space="preserve">nama satu</t>
   </si>
   <si>
     <t xml:space="preserve">Laki-laki</t>
   </si>
   <si>
-    <t xml:space="preserve">wildan@mail.com</t>
+    <t xml:space="preserve">satu@mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">qwer</t>
   </si>
   <si>
-    <t xml:space="preserve">xin zhao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xin@mail.com</t>
+    <t xml:space="preserve">nama dua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dua@mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">1234q</t>
   </si>
   <si>
-    <t xml:space="preserve">tia esport</t>
+    <t xml:space="preserve">nama tiga</t>
   </si>
   <si>
     <t xml:space="preserve">perempuan</t>
   </si>
   <si>
-    <t xml:space="preserve">tia@mail.com</t>
+    <t xml:space="preserve">tiga@mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">qw21</t>
@@ -172,10 +172,10 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.33"/>
@@ -252,9 +252,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="wildan@mail.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="xin@mail.com"/>
-    <hyperlink ref="D4" r:id="rId3" display="tia@mail.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="satu@mail.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="dua@mail.com"/>
+    <hyperlink ref="D4" r:id="rId3" display="tiga@mail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>